<commit_message>
Final training and evaluation
final_model and model .pth are not committed for swin and deit
</commit_message>
<xml_diff>
--- a/Project/code/intermediate/models/CaiT_transformer_training_run.xlsx
+++ b/Project/code/intermediate/models/CaiT_transformer_training_run.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guilh\OneDrive - Universidade de Lisboa\FCUL\2 Semestre\AP\fcul-deep-learning\Project\code\intermediate\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424D5C1A-9FAD-4B8D-BB1E-62C0652FA969}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A695EF25-07A7-4939-9F55-DC25265FB06A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="1530" windowWidth="21600" windowHeight="11715" xr2:uid="{4493D82B-8A37-4B1F-8C2B-6BB325236619}"/>
+    <workbookView xWindow="5760" yWindow="1740" windowWidth="21600" windowHeight="11715" xr2:uid="{4493D82B-8A37-4B1F-8C2B-6BB325236619}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -559,7 +559,7 @@
   <dimension ref="A1:AH6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="K2" sqref="K2:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,10 +697,10 @@
         <v>100</v>
       </c>
       <c r="J2">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="K2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L2">
         <v>1</v>
@@ -792,10 +792,10 @@
         <v>100</v>
       </c>
       <c r="J3">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="K3">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -887,10 +887,10 @@
         <v>100</v>
       </c>
       <c r="J4">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="K4">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L4">
         <v>1</v>
@@ -982,10 +982,10 @@
         <v>100</v>
       </c>
       <c r="J5">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="K5">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -1077,10 +1077,10 @@
         <v>100</v>
       </c>
       <c r="J6">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="K6">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="L6">
         <v>1</v>

</xml_diff>